<commit_message>
Updated employee processing pipelines and outputs
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,10 +496,8 @@
           <t>m.johnson@email.com</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>6145551234</t>
-        </is>
+      <c r="E2" t="n">
+        <v>6145551234</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -508,6 +506,328 @@
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Martinez</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1992-11-05</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>j.martinez@email.com</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>6195559876</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>marketing specialist</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Martinez</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1992-11-05</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>j.martinez@email.com</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>6195559876</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>marketing specialist</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Natalie</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1988-05-29</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>n.brown@email.com</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>3035552468</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>administrative assistant</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Johnson</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1990-07-22</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>m.johnson@email.com</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>6145551234</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>customer service rep</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Martinez</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1992-11-05</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>j.martinez@email.com</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>6195559876</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>marketing specialist</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Natalie</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1988-05-29</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>n.brown@email.com</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>3035552468</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>administrative assistant</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Robert</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Anderson</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1976-09-10</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>r.anderson@email.com</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>6125556789</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>project manager</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Robert</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Anderson</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1976-09-10</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>r.anderson@email.com</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>6125556789</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>project manager</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Robert</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Anderson</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1976-09-10</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>r.anderson@email.com</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>6125556789</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>project manager</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Robert</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Anderson</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1976-09-10</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>r.anderson@email.com</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>6125556789</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>project manager</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>